<commit_message>
CNN's runned as well as Otimized for Age (best with SGD)
</commit_message>
<xml_diff>
--- a/Project/Project/docs e txt/resultados.xlsx
+++ b/Project/Project/docs e txt/resultados.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulisboa-my.sharepoint.com/personal/fc59451_alunos_fc_ul_pt/Documents/MCD/2º Semestre/A.A.A/AAA_repo/Project/Project/docs e txt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D074019A-9650-4A76-9A54-1A5411831B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{D074019A-9650-4A76-9A54-1A5411831B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9EE8991-87BE-4309-A9F4-5274F4B35CB7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC6C8A81-F9E4-4394-9C0E-1907BD7675F2}"/>
+    <workbookView minimized="1" xWindow="-16875" yWindow="510" windowWidth="12150" windowHeight="20745" activeTab="1" xr2:uid="{CC6C8A81-F9E4-4394-9C0E-1907BD7675F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Unbalanced" sheetId="1" r:id="rId1"/>
+    <sheet name="Balanced" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="14">
   <si>
     <t>ACC</t>
   </si>
@@ -76,6 +77,9 @@
   <si>
     <t>Gender (Sorted by MCC)</t>
   </si>
+  <si>
+    <t>B</t>
+  </si>
 </sst>
 </file>
 
@@ -98,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +112,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,20 +149,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -251,7 +262,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Unbalanced!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -272,7 +283,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$F$3:$G$12</c:f>
+              <c:f>Unbalanced!$F$3:$G$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="10"/>
                 <c:lvl>
@@ -344,7 +355,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$12</c:f>
+              <c:f>Unbalanced!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -392,7 +403,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$2</c:f>
+              <c:f>Unbalanced!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -413,7 +424,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$F$3:$G$12</c:f>
+              <c:f>Unbalanced!$F$3:$G$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="10"/>
                 <c:lvl>
@@ -485,7 +496,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$12</c:f>
+              <c:f>Unbalanced!$I$3:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -805,7 +816,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$2</c:f>
+              <c:f>Unbalanced!$R$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -826,7 +837,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$P$3:$Q$12</c:f>
+              <c:f>Unbalanced!$P$3:$Q$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="10"/>
                 <c:lvl>
@@ -898,7 +909,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$3:$R$12</c:f>
+              <c:f>Unbalanced!$R$3:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -946,7 +957,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$2</c:f>
+              <c:f>Unbalanced!$S$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -967,7 +978,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$P$3:$Q$12</c:f>
+              <c:f>Unbalanced!$P$3:$Q$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="10"/>
                 <c:lvl>
@@ -1039,7 +1050,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$3:$S$12</c:f>
+              <c:f>Unbalanced!$S$3:$S$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2740,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183104E3-5735-4ED1-970C-896521CAAF1F}">
   <dimension ref="E1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,19 +2769,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E1" s="5"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="P1" s="4" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="P1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="5:19" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
@@ -2799,28 +2810,28 @@
       </c>
     </row>
     <row r="3" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>0.66</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="4">
         <v>0.51</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="4">
         <v>0.89</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="4">
         <v>0.78</v>
       </c>
     </row>
@@ -2837,16 +2848,16 @@
       <c r="I4" s="2">
         <v>0.42</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="4">
         <v>0.89</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="4">
         <v>0.78</v>
       </c>
     </row>
@@ -3070,4 +3081,290 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA731D09-1145-41F7-9FB7-9DE9A2C3F06B}">
+  <dimension ref="A1:T12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="Q1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.51</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="Q4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="T4" s="7">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="Q6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="Q7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="Q10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="Q1:T1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>